<commit_message>
Fixed bugs + added more instructions
</commit_message>
<xml_diff>
--- a/processor_isa.xlsx
+++ b/processor_isa.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\CPU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\CPU\4Vin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBCA8C0-E5BA-4FF9-8510-A55BD1029EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C726AD40-DE36-461A-B731-E564B99D2649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5850" yWindow="2790" windowWidth="24915" windowHeight="11385" xr2:uid="{94061592-5FFC-42D8-A5F7-A86345E201E8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="117">
   <si>
     <t>0000 0000</t>
   </si>
@@ -378,6 +378,15 @@
   </si>
   <si>
     <t>color reg/val</t>
+  </si>
+  <si>
+    <t>0x33</t>
+  </si>
+  <si>
+    <t>0011 0011</t>
+  </si>
+  <si>
+    <t>XOR</t>
   </si>
 </sst>
 </file>
@@ -735,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECE643FD-DD39-4FC1-84A2-B0C703F408E1}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,101 +1191,112 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36" t="s">
-        <v>58</v>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C37" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C41" t="s">
-        <v>100</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>61</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>107</v>
-      </c>
-      <c r="C45" t="s">
-        <v>109</v>
-      </c>
-      <c r="D45" t="s">
-        <v>111</v>
-      </c>
-      <c r="E45" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" t="s">
+        <v>109</v>
+      </c>
+      <c r="D46" t="s">
+        <v>111</v>
+      </c>
+      <c r="E46" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>110</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>108</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>84</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E47" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>41</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>42</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>84</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed memory reading/writing bugs
</commit_message>
<xml_diff>
--- a/processor_isa.xlsx
+++ b/processor_isa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\CPU\4Vin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C726AD40-DE36-461A-B731-E564B99D2649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8769B9E-815E-4804-B0F1-8CC338524704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5850" yWindow="2790" windowWidth="24915" windowHeight="11385" xr2:uid="{94061592-5FFC-42D8-A5F7-A86345E201E8}"/>
   </bookViews>
@@ -746,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECE643FD-DD39-4FC1-84A2-B0C703F408E1}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>